<commit_message>
Working on sell_profit report
</commit_message>
<xml_diff>
--- a/application/views/plugins/reports/Summary_sell_profit/Summary_sell_profit.xlsx
+++ b/application/views/plugins/reports/Summary_sell_profit/Summary_sell_profit.xlsx
@@ -14,11 +14,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+  <si>
+    <t>Всего</t>
+  </si>
   <si>
     <t>Группа</t>
   </si>
   <si>
+    <t>{$v-&gt;total_sell}</t>
+  </si>
+  <si>
     <t>{$v-&gt;rows[]-&gt;product_code}</t>
   </si>
   <si>
@@ -52,6 +58,15 @@
     <t>Ср. цена</t>
   </si>
   <si>
+    <t>{$v-&gt;total_qty}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;total_self}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;total_net}</t>
+  </si>
+  <si>
     <t>Анализ продаж и прибыли</t>
   </si>
   <si>
@@ -89,13 +104,16 @@
   </si>
   <si>
     <t>{$v-&gt;totals[]-&gt;net_sum}</t>
+  </si>
+  <si>
+    <t>Итоги</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,8 +154,17 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,8 +183,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -273,7 +306,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
@@ -286,11 +332,54 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -303,10 +392,34 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -316,7 +429,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -333,7 +446,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -360,31 +473,54 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -690,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J9"/>
+  <dimension ref="B1:J12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +844,7 @@
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -721,77 +857,77 @@
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
-        <v>0</v>
+      <c r="B4" s="17" t="s">
+        <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J4" s="10"/>
     </row>
     <row r="5" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>13</v>
-      </c>
       <c r="F5" s="11" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -805,46 +941,85 @@
       <c r="I6" s="2"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E8" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="22" t="s">
-        <v>10</v>
-      </c>
+    <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="2:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E8" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="32"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E9" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="25" t="s">
-        <v>23</v>
+      <c r="E9" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="23"/>
+      <c r="G9" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>11</v>
       </c>
       <c r="J9" s="25" t="s">
-        <v>24</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E10" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="27"/>
+      <c r="G10" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E11" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="21"/>
+      <c r="G11" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="1"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="E8:F8"/>
+  <mergeCells count="9">
     <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E8:J8"/>
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="H3:I3"/>

</xml_diff>

<commit_message>
profit report switch totals with main table
</commit_message>
<xml_diff>
--- a/application/views/plugins/reports/Summary_sell_profit/Summary_sell_profit.xlsx
+++ b/application/views/plugins/reports/Summary_sell_profit/Summary_sell_profit.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -67,9 +67,6 @@
     <t>{$v-&gt;total_net}</t>
   </si>
   <si>
-    <t>Анализ продаж и прибыли</t>
-  </si>
-  <si>
     <t>{$v-&gt;rows[]-&gt;sell_qty}</t>
   </si>
   <si>
@@ -100,13 +97,16 @@
     <t>{$v-&gt;totals[]-&gt;net_sum}</t>
   </si>
   <si>
-    <t>Итоги</t>
-  </si>
-  <si>
     <t>{$v-&gt;rows[]-&gt;group_by}</t>
   </si>
   <si>
     <t>{$v-&gt;totals[]-&gt;group_by}&lt;merge2&gt;</t>
+  </si>
+  <si>
+    <t>Итоги анализа продаж и прибыли</t>
+  </si>
+  <si>
+    <t>Развернутый анализ продаж и прибыли</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -617,7 +617,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -829,7 +829,7 @@
   <dimension ref="B1:J12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,99 +842,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="28"/>
+    <row r="2" spans="2:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E2" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31" t="s">
+      <c r="E3" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="18"/>
+      <c r="G3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31" t="s">
+      <c r="I3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="31"/>
-      <c r="J3" s="32" t="s">
+      <c r="J3" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="32"/>
+      <c r="E4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="5" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>22</v>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E5" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="20"/>
+      <c r="G5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="E6" s="1"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -942,72 +915,99 @@
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="2:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E8" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="25"/>
+    <row r="8" spans="2:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="28"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E9" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="13" t="s">
+      <c r="B9" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="30"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="G9" s="31"/>
+      <c r="H9" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="I9" s="31"/>
+      <c r="J9" s="32" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>16</v>
-      </c>
+      <c r="B10" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="32"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E11" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>26</v>
+    <row r="11" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -1016,15 +1016,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E2:J2"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="J9:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>